<commit_message>
added complex json file to excel convert
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>name</t>
   </si>
@@ -20,6 +20,9 @@
   </si>
   <si>
     <t>address</t>
+  </si>
+  <si>
+    <t>city.name</t>
   </si>
   <si>
     <t>Adib</t>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,27 +430,33 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>